<commit_message>
Removed .env from Git tracking and added to .gitignore
</commit_message>
<xml_diff>
--- a/Threats_18_Jun_2025.xlsx
+++ b/Threats_18_Jun_2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Saanvi\Downloads\only_updated_threat_mapper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{432AA81D-41B2-4DDE-ACB4-83962E5A0519}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED87D570-5D0F-4B6A-82BD-4C8940757E7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1B4D1AB6-0EDA-4D5A-A5E0-2A96E8E32D0D}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Id</t>
   </si>
@@ -50,36 +50,6 @@
   </si>
   <si>
     <t>Vcenter may be able to impersonate the context of Switch in order to gain additional privilege.</t>
-  </si>
-  <si>
-    <t>Replay Attacks</t>
-  </si>
-  <si>
-    <t>Tampering</t>
-  </si>
-  <si>
-    <t>Workstation to Firewall</t>
-  </si>
-  <si>
-    <t>Packets or messages without sequence numbers or timestamps can be captured and replayed...</t>
-  </si>
-  <si>
-    <t>Server Process Memory Tampered</t>
-  </si>
-  <si>
-    <t>Server to OS ESXi</t>
-  </si>
-  <si>
-    <t>If Server is given access to memory... then Server can tamper with OS ESXi...</t>
-  </si>
-  <si>
-    <t>NTP Process Memory Tampered</t>
-  </si>
-  <si>
-    <t>NTP to BR Solution</t>
-  </si>
-  <si>
-    <t>If NTP is given access to memory... then NTP can tamper with BR Solution...</t>
   </si>
 </sst>
 </file>
@@ -940,10 +910,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9011A7B-57E1-4202-A097-4635B5818F7B}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -985,57 +955,6 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>82</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>86</v>
-      </c>
-      <c r="B4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>91</v>
-      </c>
-      <c r="B5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" t="s">
-        <v>18</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>